<commit_message>
better fix with tests
</commit_message>
<xml_diff>
--- a/iaso/tests/fixtures/test_form_deduplication.xlsx
+++ b/iaso/tests/fixtures/test_form_deduplication.xlsx
@@ -1,20 +1,29 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10608"/>
+  <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/beygorghor/WORK/BLSQ/iaso/iaso/iaso/tests/fixtures/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{40374B8A-C643-8945-80D8-2941FDB06C5D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="40" windowWidth="15960" windowHeight="18080"/>
+    <workbookView xWindow="-21940" yWindow="-2780" windowWidth="18480" windowHeight="15020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="survey" sheetId="1" r:id="rId4"/>
-    <sheet name="choices" sheetId="2" r:id="rId5"/>
-    <sheet name="settings" sheetId="3" r:id="rId6"/>
-    <sheet name="warnings" sheetId="4" r:id="rId7"/>
+    <sheet name="survey" sheetId="1" r:id="rId1"/>
+    <sheet name="choices" sheetId="2" r:id="rId2"/>
+    <sheet name="settings" sheetId="3" r:id="rId3"/>
+    <sheet name="warnings" sheetId="4" r:id="rId4"/>
   </sheets>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="43">
   <si>
     <t>type</t>
   </si>
@@ -122,28 +131,36 @@
   </si>
   <si>
     <t>message</t>
+  </si>
+  <si>
+    <t>birth_date__date__</t>
+  </si>
+  <si>
+    <t>appointment_time__time__</t>
+  </si>
+  <si>
+    <t>Appointment time</t>
+  </si>
+  <si>
+    <t>last_update__datetime__</t>
+  </si>
+  <si>
+    <t>Last update</t>
+  </si>
+  <si>
+    <t>Birthday date</t>
+  </si>
+  <si>
+    <t>2024-06-11T14:30:00</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
-    <numFmt numFmtId="0" formatCode="General"/>
-  </numFmts>
-  <fonts count="4">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
-      <color indexed="8"/>
-      <name val="Calibri"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color indexed="8"/>
-      <name val="Helvetica Neue"/>
-    </font>
-    <font>
-      <sz val="15"/>
       <color indexed="8"/>
       <name val="Calibri"/>
     </font>
@@ -151,6 +168,13 @@
       <sz val="10"/>
       <color indexed="8"/>
       <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color indexed="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="3">
@@ -229,53 +253,24 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
-    <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
+  <cellXfs count="15">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="20" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -284,24 +279,85 @@
   <tableStyles count="0"/>
   <colors>
     <indexedColors>
-      <rgbColor rgb="ff000000"/>
-      <rgbColor rgb="ffffffff"/>
-      <rgbColor rgb="ffff0000"/>
-      <rgbColor rgb="ff00ff00"/>
-      <rgbColor rgb="ff0000ff"/>
-      <rgbColor rgb="ffffff00"/>
-      <rgbColor rgb="ffff00ff"/>
-      <rgbColor rgb="ff00ffff"/>
-      <rgbColor rgb="ff000000"/>
-      <rgbColor rgb="ffffffff"/>
-      <rgbColor rgb="ffaaaaaa"/>
+      <rgbColor rgb="FF000000"/>
+      <rgbColor rgb="FFFFFFFF"/>
+      <rgbColor rgb="FFFF0000"/>
+      <rgbColor rgb="FF00FF00"/>
+      <rgbColor rgb="FF0000FF"/>
+      <rgbColor rgb="FFFFFF00"/>
+      <rgbColor rgb="FFFF00FF"/>
+      <rgbColor rgb="FF00FFFF"/>
+      <rgbColor rgb="FF000000"/>
+      <rgbColor rgb="FFFFFFFF"/>
+      <rgbColor rgb="FFAAAAAA"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
     </indexedColors>
   </colors>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office Theme">
       <a:dk1>
@@ -427,7 +483,7 @@
       <a:effectStyleLst>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw sx="100000" sy="100000" kx="0" ky="0" algn="b" rotWithShape="0" blurRad="38100" dist="23000" dir="5400000">
+            <a:outerShdw blurRad="38100" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -436,7 +492,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw sx="100000" sy="100000" kx="0" ky="0" algn="b" rotWithShape="0" blurRad="38100" dist="23000" dir="5400000">
+            <a:outerShdw blurRad="38100" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -445,7 +501,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw sx="100000" sy="100000" kx="0" ky="0" algn="b" rotWithShape="0" blurRad="38100" dist="23000" dir="5400000">
+            <a:outerShdw blurRad="38100" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -519,7 +575,7 @@
           <a:round/>
         </a:ln>
         <a:effectLst>
-          <a:outerShdw sx="100000" sy="100000" kx="0" ky="0" algn="b" rotWithShape="0" blurRad="38100" dist="23000" dir="5400000">
+          <a:outerShdw blurRad="38100" dist="23000" dir="5400000" rotWithShape="0">
             <a:srgbClr val="000000">
               <a:alpha val="35000"/>
             </a:srgbClr>
@@ -527,7 +583,7 @@
         </a:effectLst>
         <a:sp3d/>
       </a:spPr>
-      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="45718" tIns="45718" rIns="45718" bIns="45718" numCol="1" spcCol="38100" rtlCol="0" anchor="ctr" upright="0">
+      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="45718" tIns="45718" rIns="45718" bIns="45718" numCol="1" spcCol="38100" rtlCol="0" anchor="ctr">
         <a:spAutoFit/>
       </a:bodyPr>
       <a:lstStyle>
@@ -545,7 +601,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1100" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1100" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -574,7 +630,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -599,7 +655,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -624,7 +680,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -649,7 +705,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -674,7 +730,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -699,7 +755,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -724,7 +780,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -749,7 +805,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -774,7 +830,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -787,9 +843,15 @@
         </a:lvl9pPr>
       </a:lstStyle>
       <a:style>
-        <a:lnRef idx="0"/>
-        <a:fillRef idx="0"/>
-        <a:effectRef idx="0"/>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
         <a:fontRef idx="none"/>
       </a:style>
     </a:spDef>
@@ -804,7 +866,7 @@
           <a:round/>
         </a:ln>
         <a:effectLst>
-          <a:outerShdw sx="100000" sy="100000" kx="0" ky="0" algn="b" rotWithShape="0" blurRad="38100" dist="23000" dir="5400000">
+          <a:outerShdw blurRad="38100" dist="23000" dir="5400000" rotWithShape="0">
             <a:srgbClr val="000000">
               <a:alpha val="35000"/>
             </a:srgbClr>
@@ -812,7 +874,7 @@
         </a:effectLst>
         <a:sp3d/>
       </a:spPr>
-      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="91439" tIns="45719" rIns="91439" bIns="45719" numCol="1" spcCol="38100" rtlCol="0" anchor="t" upright="0">
+      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="91439" tIns="45719" rIns="91439" bIns="45719" numCol="1" spcCol="38100" rtlCol="0" anchor="t">
         <a:noAutofit/>
       </a:bodyPr>
       <a:lstStyle>
@@ -830,7 +892,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -855,7 +917,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -880,7 +942,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -905,7 +967,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -930,7 +992,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -955,7 +1017,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -980,7 +1042,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1005,7 +1067,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1030,7 +1092,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1055,7 +1117,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1068,9 +1130,15 @@
         </a:lvl9pPr>
       </a:lstStyle>
       <a:style>
-        <a:lnRef idx="0"/>
-        <a:fillRef idx="0"/>
-        <a:effectRef idx="0"/>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
         <a:fontRef idx="none"/>
       </a:style>
     </a:lnDef>
@@ -1084,7 +1152,7 @@
         <a:effectLst/>
         <a:sp3d/>
       </a:spPr>
-      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="45718" tIns="45718" rIns="45718" bIns="45718" numCol="1" spcCol="38100" rtlCol="0" anchor="t" upright="0">
+      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="45718" tIns="45718" rIns="45718" bIns="45718" numCol="1" spcCol="38100" rtlCol="0" anchor="t">
         <a:spAutoFit/>
       </a:bodyPr>
       <a:lstStyle>
@@ -1102,7 +1170,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1100" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1100" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1131,7 +1199,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1156,7 +1224,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1181,7 +1249,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1206,7 +1274,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1231,7 +1299,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1256,7 +1324,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1281,7 +1349,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1306,7 +1374,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1331,7 +1399,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1344,72 +1412,81 @@
         </a:lvl9pPr>
       </a:lstStyle>
       <a:style>
-        <a:lnRef idx="0"/>
-        <a:fillRef idx="0"/>
-        <a:effectRef idx="0"/>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
         <a:fontRef idx="none"/>
       </a:style>
     </a:txDef>
   </a:objectDefaults>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:I10"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:I12"/>
   <sheetViews>
-    <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="C15" sqref="C15"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.8333" defaultRowHeight="16" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="10.8516" style="1" customWidth="1"/>
-    <col min="2" max="2" width="33.3516" style="1" customWidth="1"/>
-    <col min="3" max="4" width="16.6719" style="1" customWidth="1"/>
-    <col min="5" max="9" width="10.8516" style="1" customWidth="1"/>
-    <col min="10" max="16384" width="10.8516" style="1" customWidth="1"/>
+    <col min="1" max="1" width="10.83203125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="33.33203125" style="1" customWidth="1"/>
+    <col min="3" max="4" width="16.6640625" style="1" customWidth="1"/>
+    <col min="5" max="10" width="10.83203125" style="1" customWidth="1"/>
+    <col min="11" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="15.35" customHeight="1">
-      <c r="A1" t="s" s="2">
+    <row r="1" spans="1:9" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s" s="2">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s" s="2">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s" s="2">
+      <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s" s="2">
+      <c r="E1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s" s="2">
+      <c r="F1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="G1" t="s" s="2">
+      <c r="G1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="H1" t="s" s="2">
+      <c r="H1" s="2" t="s">
         <v>7</v>
       </c>
       <c r="I1" s="2"/>
     </row>
-    <row r="2" ht="15.35" customHeight="1">
-      <c r="A2" t="s" s="2">
+    <row r="2" spans="1:9" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="B2" t="s" s="2">
+      <c r="B2" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="C2" t="s" s="2">
+      <c r="C2" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="D2" t="s" s="2">
+      <c r="D2" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="E2" t="s" s="2">
+      <c r="E2" s="2" t="s">
         <v>10</v>
       </c>
       <c r="F2" s="3"/>
@@ -1417,20 +1494,20 @@
       <c r="H2" s="3"/>
       <c r="I2" s="3"/>
     </row>
-    <row r="3" ht="15.35" customHeight="1">
-      <c r="A3" t="s" s="2">
+    <row r="3" spans="1:9" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="B3" t="s" s="2">
+      <c r="B3" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="C3" t="s" s="2">
+      <c r="C3" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="D3" t="s" s="2">
+      <c r="D3" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="E3" t="s" s="2">
+      <c r="E3" s="2" t="s">
         <v>10</v>
       </c>
       <c r="F3" s="3"/>
@@ -1438,17 +1515,17 @@
       <c r="H3" s="3"/>
       <c r="I3" s="3"/>
     </row>
-    <row r="4" ht="15.35" customHeight="1">
-      <c r="A4" t="s" s="2">
+    <row r="4" spans="1:9" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="B4" t="s" s="2">
+      <c r="B4" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="C4" t="s" s="2">
+      <c r="C4" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="D4" t="s" s="2">
+      <c r="D4" s="2" t="s">
         <v>14</v>
       </c>
       <c r="E4" s="3"/>
@@ -1459,17 +1536,17 @@
       </c>
       <c r="I4" s="3"/>
     </row>
-    <row r="5" ht="15.35" customHeight="1">
-      <c r="A5" t="s" s="2">
+    <row r="5" spans="1:9" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="B5" t="s" s="2">
+      <c r="B5" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="C5" t="s" s="2">
+      <c r="C5" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="D5" t="s" s="2">
+      <c r="D5" s="2" t="s">
         <v>16</v>
       </c>
       <c r="E5" s="3"/>
@@ -1480,17 +1557,17 @@
       </c>
       <c r="I5" s="3"/>
     </row>
-    <row r="6" ht="15.35" customHeight="1">
-      <c r="A6" t="s" s="2">
+    <row r="6" spans="1:9" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="B6" t="s" s="2">
+      <c r="B6" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="C6" t="s" s="2">
+      <c r="C6" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="D6" t="s" s="2">
+      <c r="D6" s="2" t="s">
         <v>18</v>
       </c>
       <c r="E6" s="3"/>
@@ -1501,17 +1578,17 @@
       </c>
       <c r="I6" s="3"/>
     </row>
-    <row r="7" ht="13.65" customHeight="1">
-      <c r="A7" t="s" s="5">
+    <row r="7" spans="1:9" ht="13.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="B7" t="s" s="5">
+      <c r="B7" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="C7" t="s" s="5">
+      <c r="C7" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="D7" t="s" s="5">
+      <c r="D7" s="5" t="s">
         <v>20</v>
       </c>
       <c r="E7" s="6"/>
@@ -1522,28 +1599,322 @@
       </c>
       <c r="I7" s="6"/>
     </row>
-    <row r="8" ht="15.35" customHeight="1">
-      <c r="A8" t="s" s="2">
+    <row r="8" spans="1:9" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="B8" t="s" s="2">
+      <c r="B8" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="C8" t="s" s="2">
+      <c r="C8" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="D8" t="s" s="2">
+      <c r="D8" s="2" t="s">
         <v>22</v>
       </c>
       <c r="E8" s="3"/>
       <c r="F8" s="3"/>
       <c r="G8" s="3"/>
-      <c r="H8" t="s" s="2">
+      <c r="H8" s="2" t="s">
         <v>23</v>
       </c>
       <c r="I8" s="3"/>
     </row>
-    <row r="9" ht="15.35" customHeight="1">
+    <row r="9" spans="1:9" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="C9" s="11" t="s">
+        <v>41</v>
+      </c>
+      <c r="D9" s="11" t="s">
+        <v>41</v>
+      </c>
+      <c r="E9" s="3"/>
+      <c r="F9" s="3"/>
+      <c r="G9" s="3"/>
+      <c r="H9" s="13">
+        <v>32874</v>
+      </c>
+      <c r="I9" s="3"/>
+    </row>
+    <row r="10" spans="1:9" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="C10" s="12" t="s">
+        <v>38</v>
+      </c>
+      <c r="D10" s="12" t="s">
+        <v>38</v>
+      </c>
+      <c r="E10" s="3"/>
+      <c r="F10" s="3"/>
+      <c r="G10" s="3"/>
+      <c r="H10" s="14">
+        <v>0.60416666666666663</v>
+      </c>
+      <c r="I10" s="3"/>
+    </row>
+    <row r="11" spans="1:9" s="3" customFormat="1" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A11" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="C11" s="11" t="s">
+        <v>40</v>
+      </c>
+      <c r="D11" s="11" t="s">
+        <v>40</v>
+      </c>
+      <c r="H11" s="7" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A12" s="8"/>
+      <c r="B12" s="9"/>
+      <c r="C12" s="9"/>
+      <c r="D12" s="9"/>
+      <c r="E12" s="9"/>
+      <c r="F12" s="9"/>
+      <c r="G12" s="10"/>
+      <c r="H12" s="3"/>
+      <c r="I12" s="3"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait"/>
+  <headerFooter>
+    <oddFooter>&amp;C&amp;"Helvetica Neue,Regular"&amp;12&amp;K000000&amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:E10"/>
+  <sheetViews>
+    <sheetView showGridLines="0" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16" customHeight="1" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="6" width="10.83203125" style="1" customWidth="1"/>
+    <col min="7" max="16384" width="10.83203125" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="3"/>
+      <c r="E1" s="3"/>
+    </row>
+    <row r="2" spans="1:5" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="3"/>
+      <c r="B2" s="3"/>
+      <c r="C2" s="3"/>
+      <c r="D2" s="3"/>
+      <c r="E2" s="3"/>
+    </row>
+    <row r="3" spans="1:5" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="3"/>
+      <c r="B3" s="3"/>
+      <c r="C3" s="3"/>
+      <c r="D3" s="3"/>
+      <c r="E3" s="3"/>
+    </row>
+    <row r="4" spans="1:5" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="3"/>
+      <c r="B4" s="3"/>
+      <c r="C4" s="3"/>
+      <c r="D4" s="3"/>
+      <c r="E4" s="3"/>
+    </row>
+    <row r="5" spans="1:5" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="3"/>
+      <c r="B5" s="3"/>
+      <c r="C5" s="3"/>
+      <c r="D5" s="3"/>
+      <c r="E5" s="3"/>
+    </row>
+    <row r="6" spans="1:5" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="3"/>
+      <c r="B6" s="3"/>
+      <c r="C6" s="3"/>
+      <c r="D6" s="3"/>
+      <c r="E6" s="3"/>
+    </row>
+    <row r="7" spans="1:5" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="3"/>
+      <c r="B7" s="3"/>
+      <c r="C7" s="3"/>
+      <c r="D7" s="3"/>
+      <c r="E7" s="3"/>
+    </row>
+    <row r="8" spans="1:5" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="3"/>
+      <c r="B8" s="3"/>
+      <c r="C8" s="3"/>
+      <c r="D8" s="3"/>
+      <c r="E8" s="3"/>
+    </row>
+    <row r="9" spans="1:5" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="3"/>
+      <c r="B9" s="3"/>
+      <c r="C9" s="3"/>
+      <c r="D9" s="3"/>
+      <c r="E9" s="3"/>
+    </row>
+    <row r="10" spans="1:5" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="3"/>
+      <c r="B10" s="3"/>
+      <c r="C10" s="3"/>
+      <c r="D10" s="3"/>
+      <c r="E10" s="3"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait"/>
+  <headerFooter>
+    <oddFooter>&amp;C&amp;"Helvetica Neue,Regular"&amp;12&amp;K000000&amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+  <dimension ref="A1:H10"/>
+  <sheetViews>
+    <sheetView showGridLines="0" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16" customHeight="1" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="9" width="10.83203125" style="1" customWidth="1"/>
+    <col min="10" max="16384" width="10.83203125" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="C2" s="3"/>
+      <c r="D2" s="3"/>
+      <c r="E2" s="3"/>
+      <c r="F2" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="H2" s="4">
+        <v>1680182012</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="3"/>
+      <c r="B3" s="3"/>
+      <c r="C3" s="3"/>
+      <c r="D3" s="3"/>
+      <c r="E3" s="3"/>
+      <c r="F3" s="3"/>
+      <c r="G3" s="3"/>
+      <c r="H3" s="3"/>
+    </row>
+    <row r="4" spans="1:8" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="3"/>
+      <c r="B4" s="3"/>
+      <c r="C4" s="3"/>
+      <c r="D4" s="3"/>
+      <c r="E4" s="3"/>
+      <c r="F4" s="3"/>
+      <c r="G4" s="3"/>
+      <c r="H4" s="3"/>
+    </row>
+    <row r="5" spans="1:8" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="3"/>
+      <c r="B5" s="3"/>
+      <c r="C5" s="3"/>
+      <c r="D5" s="3"/>
+      <c r="E5" s="3"/>
+      <c r="F5" s="3"/>
+      <c r="G5" s="3"/>
+      <c r="H5" s="3"/>
+    </row>
+    <row r="6" spans="1:8" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="3"/>
+      <c r="B6" s="3"/>
+      <c r="C6" s="3"/>
+      <c r="D6" s="3"/>
+      <c r="E6" s="3"/>
+      <c r="F6" s="3"/>
+      <c r="G6" s="3"/>
+      <c r="H6" s="3"/>
+    </row>
+    <row r="7" spans="1:8" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="3"/>
+      <c r="B7" s="3"/>
+      <c r="C7" s="3"/>
+      <c r="D7" s="3"/>
+      <c r="E7" s="3"/>
+      <c r="F7" s="3"/>
+      <c r="G7" s="3"/>
+      <c r="H7" s="3"/>
+    </row>
+    <row r="8" spans="1:8" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="3"/>
+      <c r="B8" s="3"/>
+      <c r="C8" s="3"/>
+      <c r="D8" s="3"/>
+      <c r="E8" s="3"/>
+      <c r="F8" s="3"/>
+      <c r="G8" s="3"/>
+      <c r="H8" s="3"/>
+    </row>
+    <row r="9" spans="1:8" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="3"/>
       <c r="B9" s="3"/>
       <c r="C9" s="3"/>
@@ -1552,254 +1923,8 @@
       <c r="F9" s="3"/>
       <c r="G9" s="3"/>
       <c r="H9" s="3"/>
-      <c r="I9" s="3"/>
-    </row>
-    <row r="10" ht="15.35" customHeight="1">
-      <c r="A10" s="8"/>
-      <c r="B10" s="9"/>
-      <c r="C10" s="9"/>
-      <c r="D10" s="9"/>
-      <c r="E10" s="9"/>
-      <c r="F10" s="9"/>
-      <c r="G10" s="10"/>
-      <c r="H10" s="3"/>
-      <c r="I10" s="3"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup firstPageNumber="1" fitToHeight="1" fitToWidth="1" scale="100" useFirstPageNumber="0" orientation="portrait" pageOrder="downThenOver"/>
-  <headerFooter>
-    <oddFooter>&amp;C&amp;"Helvetica Neue,Regular"&amp;12&amp;K000000&amp;P</oddFooter>
-  </headerFooter>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:E10"/>
-  <sheetViews>
-    <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="10.8333" defaultRowHeight="16" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
-  <cols>
-    <col min="1" max="5" width="10.8516" style="11" customWidth="1"/>
-    <col min="6" max="16384" width="10.8516" style="11" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" ht="15.35" customHeight="1">
-      <c r="A1" t="s" s="2">
-        <v>24</v>
-      </c>
-      <c r="B1" t="s" s="2">
-        <v>1</v>
-      </c>
-      <c r="C1" t="s" s="2">
-        <v>2</v>
-      </c>
-      <c r="D1" s="3"/>
-      <c r="E1" s="3"/>
-    </row>
-    <row r="2" ht="15.35" customHeight="1">
-      <c r="A2" s="3"/>
-      <c r="B2" s="3"/>
-      <c r="C2" s="3"/>
-      <c r="D2" s="3"/>
-      <c r="E2" s="3"/>
-    </row>
-    <row r="3" ht="15.35" customHeight="1">
-      <c r="A3" s="3"/>
-      <c r="B3" s="3"/>
-      <c r="C3" s="3"/>
-      <c r="D3" s="3"/>
-      <c r="E3" s="3"/>
-    </row>
-    <row r="4" ht="15.35" customHeight="1">
-      <c r="A4" s="3"/>
-      <c r="B4" s="3"/>
-      <c r="C4" s="3"/>
-      <c r="D4" s="3"/>
-      <c r="E4" s="3"/>
-    </row>
-    <row r="5" ht="15.35" customHeight="1">
-      <c r="A5" s="3"/>
-      <c r="B5" s="3"/>
-      <c r="C5" s="3"/>
-      <c r="D5" s="3"/>
-      <c r="E5" s="3"/>
-    </row>
-    <row r="6" ht="15.35" customHeight="1">
-      <c r="A6" s="3"/>
-      <c r="B6" s="3"/>
-      <c r="C6" s="3"/>
-      <c r="D6" s="3"/>
-      <c r="E6" s="3"/>
-    </row>
-    <row r="7" ht="15.35" customHeight="1">
-      <c r="A7" s="3"/>
-      <c r="B7" s="3"/>
-      <c r="C7" s="3"/>
-      <c r="D7" s="3"/>
-      <c r="E7" s="3"/>
-    </row>
-    <row r="8" ht="15.35" customHeight="1">
-      <c r="A8" s="3"/>
-      <c r="B8" s="3"/>
-      <c r="C8" s="3"/>
-      <c r="D8" s="3"/>
-      <c r="E8" s="3"/>
-    </row>
-    <row r="9" ht="15.35" customHeight="1">
-      <c r="A9" s="3"/>
-      <c r="B9" s="3"/>
-      <c r="C9" s="3"/>
-      <c r="D9" s="3"/>
-      <c r="E9" s="3"/>
-    </row>
-    <row r="10" ht="15.35" customHeight="1">
-      <c r="A10" s="3"/>
-      <c r="B10" s="3"/>
-      <c r="C10" s="3"/>
-      <c r="D10" s="3"/>
-      <c r="E10" s="3"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup firstPageNumber="1" fitToHeight="1" fitToWidth="1" scale="100" useFirstPageNumber="0" orientation="portrait" pageOrder="downThenOver"/>
-  <headerFooter>
-    <oddFooter>&amp;C&amp;"Helvetica Neue,Regular"&amp;12&amp;K000000&amp;P</oddFooter>
-  </headerFooter>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:H10"/>
-  <sheetViews>
-    <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="10.8333" defaultRowHeight="16" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
-  <cols>
-    <col min="1" max="8" width="10.8516" style="12" customWidth="1"/>
-    <col min="9" max="16384" width="10.8516" style="12" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" ht="15.35" customHeight="1">
-      <c r="A1" t="s" s="2">
-        <v>25</v>
-      </c>
-      <c r="B1" t="s" s="2">
-        <v>26</v>
-      </c>
-      <c r="C1" t="s" s="2">
-        <v>27</v>
-      </c>
-      <c r="D1" t="s" s="2">
-        <v>28</v>
-      </c>
-      <c r="E1" t="s" s="2">
-        <v>29</v>
-      </c>
-      <c r="F1" t="s" s="2">
-        <v>30</v>
-      </c>
-      <c r="G1" t="s" s="2">
-        <v>31</v>
-      </c>
-      <c r="H1" t="s" s="2">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="2" ht="15.35" customHeight="1">
-      <c r="A2" t="s" s="2">
-        <v>33</v>
-      </c>
-      <c r="B2" t="s" s="2">
-        <v>34</v>
-      </c>
-      <c r="C2" s="3"/>
-      <c r="D2" s="3"/>
-      <c r="E2" s="3"/>
-      <c r="F2" t="s" s="2">
-        <v>6</v>
-      </c>
-      <c r="G2" t="s" s="2">
-        <v>6</v>
-      </c>
-      <c r="H2" s="4">
-        <v>1680182012</v>
-      </c>
-    </row>
-    <row r="3" ht="15.35" customHeight="1">
-      <c r="A3" s="3"/>
-      <c r="B3" s="3"/>
-      <c r="C3" s="3"/>
-      <c r="D3" s="3"/>
-      <c r="E3" s="3"/>
-      <c r="F3" s="3"/>
-      <c r="G3" s="3"/>
-      <c r="H3" s="3"/>
-    </row>
-    <row r="4" ht="15.35" customHeight="1">
-      <c r="A4" s="3"/>
-      <c r="B4" s="3"/>
-      <c r="C4" s="3"/>
-      <c r="D4" s="3"/>
-      <c r="E4" s="3"/>
-      <c r="F4" s="3"/>
-      <c r="G4" s="3"/>
-      <c r="H4" s="3"/>
-    </row>
-    <row r="5" ht="15.35" customHeight="1">
-      <c r="A5" s="3"/>
-      <c r="B5" s="3"/>
-      <c r="C5" s="3"/>
-      <c r="D5" s="3"/>
-      <c r="E5" s="3"/>
-      <c r="F5" s="3"/>
-      <c r="G5" s="3"/>
-      <c r="H5" s="3"/>
-    </row>
-    <row r="6" ht="15.35" customHeight="1">
-      <c r="A6" s="3"/>
-      <c r="B6" s="3"/>
-      <c r="C6" s="3"/>
-      <c r="D6" s="3"/>
-      <c r="E6" s="3"/>
-      <c r="F6" s="3"/>
-      <c r="G6" s="3"/>
-      <c r="H6" s="3"/>
-    </row>
-    <row r="7" ht="15.35" customHeight="1">
-      <c r="A7" s="3"/>
-      <c r="B7" s="3"/>
-      <c r="C7" s="3"/>
-      <c r="D7" s="3"/>
-      <c r="E7" s="3"/>
-      <c r="F7" s="3"/>
-      <c r="G7" s="3"/>
-      <c r="H7" s="3"/>
-    </row>
-    <row r="8" ht="15.35" customHeight="1">
-      <c r="A8" s="3"/>
-      <c r="B8" s="3"/>
-      <c r="C8" s="3"/>
-      <c r="D8" s="3"/>
-      <c r="E8" s="3"/>
-      <c r="F8" s="3"/>
-      <c r="G8" s="3"/>
-      <c r="H8" s="3"/>
-    </row>
-    <row r="9" ht="15.35" customHeight="1">
-      <c r="A9" s="3"/>
-      <c r="B9" s="3"/>
-      <c r="C9" s="3"/>
-      <c r="D9" s="3"/>
-      <c r="E9" s="3"/>
-      <c r="F9" s="3"/>
-      <c r="G9" s="3"/>
-      <c r="H9" s="3"/>
-    </row>
-    <row r="10" ht="15.35" customHeight="1">
+    </row>
+    <row r="10" spans="1:8" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="3"/>
       <c r="B10" s="3"/>
       <c r="C10" s="3"/>
@@ -1811,7 +1936,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup firstPageNumber="1" fitToHeight="1" fitToWidth="1" scale="100" useFirstPageNumber="0" orientation="portrait" pageOrder="downThenOver"/>
+  <pageSetup orientation="portrait"/>
   <headerFooter>
     <oddFooter>&amp;C&amp;"Helvetica Neue,Regular"&amp;12&amp;K000000&amp;P</oddFooter>
   </headerFooter>
@@ -1819,19 +1944,19 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:E10"/>
   <sheetViews>
-    <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
+    <sheetView showGridLines="0" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.8333" defaultRowHeight="16" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="5" width="10.8516" style="13" customWidth="1"/>
-    <col min="6" max="16384" width="10.8516" style="13" customWidth="1"/>
+    <col min="1" max="6" width="10.83203125" style="1" customWidth="1"/>
+    <col min="7" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="15.35" customHeight="1">
-      <c r="A1" t="s" s="2">
+    <row r="1" spans="1:5" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="2" t="s">
         <v>35</v>
       </c>
       <c r="B1" s="3"/>
@@ -1839,63 +1964,63 @@
       <c r="D1" s="3"/>
       <c r="E1" s="3"/>
     </row>
-    <row r="2" ht="15.35" customHeight="1">
+    <row r="2" spans="1:5" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="3"/>
       <c r="B2" s="3"/>
       <c r="C2" s="3"/>
       <c r="D2" s="3"/>
       <c r="E2" s="3"/>
     </row>
-    <row r="3" ht="15.35" customHeight="1">
+    <row r="3" spans="1:5" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="3"/>
       <c r="B3" s="3"/>
       <c r="C3" s="3"/>
       <c r="D3" s="3"/>
       <c r="E3" s="3"/>
     </row>
-    <row r="4" ht="15.35" customHeight="1">
+    <row r="4" spans="1:5" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="3"/>
       <c r="B4" s="3"/>
       <c r="C4" s="3"/>
       <c r="D4" s="3"/>
       <c r="E4" s="3"/>
     </row>
-    <row r="5" ht="15.35" customHeight="1">
+    <row r="5" spans="1:5" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="3"/>
       <c r="B5" s="3"/>
       <c r="C5" s="3"/>
       <c r="D5" s="3"/>
       <c r="E5" s="3"/>
     </row>
-    <row r="6" ht="15.35" customHeight="1">
+    <row r="6" spans="1:5" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="3"/>
       <c r="B6" s="3"/>
       <c r="C6" s="3"/>
       <c r="D6" s="3"/>
       <c r="E6" s="3"/>
     </row>
-    <row r="7" ht="15.35" customHeight="1">
+    <row r="7" spans="1:5" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="3"/>
       <c r="B7" s="3"/>
       <c r="C7" s="3"/>
       <c r="D7" s="3"/>
       <c r="E7" s="3"/>
     </row>
-    <row r="8" ht="15.35" customHeight="1">
+    <row r="8" spans="1:5" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="3"/>
       <c r="B8" s="3"/>
       <c r="C8" s="3"/>
       <c r="D8" s="3"/>
       <c r="E8" s="3"/>
     </row>
-    <row r="9" ht="15.35" customHeight="1">
+    <row r="9" spans="1:5" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="3"/>
       <c r="B9" s="3"/>
       <c r="C9" s="3"/>
       <c r="D9" s="3"/>
       <c r="E9" s="3"/>
     </row>
-    <row r="10" ht="15.35" customHeight="1">
+    <row r="10" spans="1:5" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="3"/>
       <c r="B10" s="3"/>
       <c r="C10" s="3"/>
@@ -1904,7 +2029,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup firstPageNumber="1" fitToHeight="1" fitToWidth="1" scale="100" useFirstPageNumber="0" orientation="portrait" pageOrder="downThenOver"/>
+  <pageSetup orientation="portrait"/>
   <headerFooter>
     <oddFooter>&amp;C&amp;"Helvetica Neue,Regular"&amp;12&amp;K000000&amp;P</oddFooter>
   </headerFooter>

</xml_diff>